<commit_message>
MNT: experimenting with KMeans and Elbow curve
</commit_message>
<xml_diff>
--- a/Resources/shopping_data_cleaned.xlsx
+++ b/Resources/shopping_data_cleaned.xlsx
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E204"/>
+  <dimension ref="A1:E201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -643,313 +643,322 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>37</v>
       </c>
       <c r="D16">
         <v>20</v>
       </c>
       <c r="E16">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D17">
         <v>20</v>
       </c>
       <c r="E17">
-        <v>13</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D18">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E18">
-        <v>79</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D19">
         <v>21</v>
       </c>
       <c r="E19">
-        <v>35</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D20">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E20">
-        <v>66</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D21">
         <v>23</v>
       </c>
       <c r="E21">
-        <v>29</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>35</v>
       </c>
       <c r="D22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E22">
-        <v>98</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D23">
         <v>24</v>
       </c>
       <c r="E23">
-        <v>35</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24">
+        <v>46</v>
+      </c>
+      <c r="D24">
         <v>25</v>
       </c>
-      <c r="D24">
-        <v>24</v>
-      </c>
       <c r="E24">
-        <v>73</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D25">
         <v>25</v>
       </c>
       <c r="E25">
-        <v>5</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="D26">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E26">
-        <v>73</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D27">
         <v>28</v>
       </c>
       <c r="E27">
-        <v>14</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D28">
         <v>28</v>
       </c>
       <c r="E28">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D29">
         <v>28</v>
       </c>
       <c r="E29">
-        <v>32</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E30">
-        <v>61</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D31">
         <v>29</v>
       </c>
       <c r="E31">
-        <v>31</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>60</v>
+      </c>
+      <c r="D32">
         <v>30</v>
       </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>23</v>
-      </c>
-      <c r="D32">
-        <v>29</v>
-      </c>
       <c r="E32">
-        <v>87</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>21</v>
       </c>
       <c r="D33">
         <v>30</v>
       </c>
+      <c r="E33">
+        <v>73</v>
+      </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D34">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E34">
         <v>4</v>
@@ -957,356 +966,356 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>18</v>
+      </c>
+      <c r="D35">
         <v>33</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <v>21</v>
-      </c>
-      <c r="D35">
-        <v>30</v>
-      </c>
       <c r="E35">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D36">
         <v>33</v>
       </c>
       <c r="E36">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D37">
         <v>33</v>
       </c>
       <c r="E37">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
       <c r="C38">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D38">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E38">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
       <c r="C39">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D39">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E39">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B40">
         <v>0</v>
       </c>
       <c r="C40">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D40">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E40">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="C41">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D41">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E41">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="C42">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="D42">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E42">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D43">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E43">
-        <v>75</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D44">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E44">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D45">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E45">
-        <v>92</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D46">
         <v>39</v>
       </c>
       <c r="E46">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
       <c r="C47">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D47">
         <v>39</v>
       </c>
       <c r="E47">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="C48">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D48">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E48">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1">
+        <v>49</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>27</v>
+      </c>
+      <c r="D49">
+        <v>40</v>
+      </c>
+      <c r="E49">
         <v>47</v>
-      </c>
-      <c r="B49">
-        <v>0</v>
-      </c>
-      <c r="C49">
-        <v>24</v>
-      </c>
-      <c r="D49">
-        <v>39</v>
-      </c>
-      <c r="E49">
-        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D50">
         <v>40</v>
       </c>
       <c r="E50">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D51">
         <v>40</v>
       </c>
       <c r="E51">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="C52">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="D52">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E52">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D53">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E53">
-        <v>42</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B54">
         <v>0</v>
       </c>
       <c r="C54">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="D54">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E54">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
       <c r="C55">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="D55">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E55">
         <v>60</v>
@@ -1314,101 +1323,101 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
       <c r="C56">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="D56">
         <v>43</v>
       </c>
       <c r="E56">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D57">
         <v>43</v>
       </c>
       <c r="E57">
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B58">
         <v>0</v>
       </c>
       <c r="C58">
+        <v>51</v>
+      </c>
+      <c r="D58">
+        <v>44</v>
+      </c>
+      <c r="E58">
         <v>50</v>
-      </c>
-      <c r="D58">
-        <v>43</v>
-      </c>
-      <c r="E58">
-        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B59">
         <v>1</v>
       </c>
       <c r="C59">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="D59">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E59">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B60">
         <v>0</v>
       </c>
       <c r="C60">
+        <v>27</v>
+      </c>
+      <c r="D60">
+        <v>46</v>
+      </c>
+      <c r="E60">
         <v>51</v>
-      </c>
-      <c r="D60">
-        <v>44</v>
-      </c>
-      <c r="E60">
-        <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B61">
         <v>1</v>
       </c>
       <c r="C61">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D61">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E61">
         <v>46</v>
@@ -1416,101 +1425,101 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C62">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D62">
         <v>46</v>
       </c>
       <c r="E62">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
       <c r="C63">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="D63">
         <v>46</v>
       </c>
       <c r="E63">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="1">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C64">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D64">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E64">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="D65">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E65">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="1">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D66">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E66">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="1">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C67">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D67">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E67">
         <v>59</v>
@@ -1518,900 +1527,900 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="1">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C68">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="D68">
         <v>48</v>
       </c>
       <c r="E68">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="1">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C69">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="D69">
         <v>48</v>
       </c>
       <c r="E69">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="1">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C70">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D70">
         <v>48</v>
       </c>
       <c r="E70">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="1">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B71">
         <v>0</v>
       </c>
       <c r="C71">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="D71">
         <v>48</v>
       </c>
       <c r="E71">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="1">
+        <v>72</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72">
         <v>70</v>
       </c>
-      <c r="B72">
-        <v>1</v>
-      </c>
-      <c r="C72">
-        <v>19</v>
-      </c>
       <c r="D72">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E72">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="1">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B73">
         <v>0</v>
       </c>
       <c r="C73">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D73">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E73">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="1">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C74">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D74">
+        <v>50</v>
+      </c>
+      <c r="E74">
         <v>49</v>
-      </c>
-      <c r="E74">
-        <v>55</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="1">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B75">
         <v>0</v>
       </c>
       <c r="C75">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="D75">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E75">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="1">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C76">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D76">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E76">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="1">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C77">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="D77">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E77">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="1">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C78">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D78">
         <v>54</v>
       </c>
       <c r="E78">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="1">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B79">
         <v>1</v>
       </c>
       <c r="C79">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D79">
         <v>54</v>
       </c>
       <c r="E79">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="1">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B80">
         <v>0</v>
       </c>
       <c r="C80">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="D80">
         <v>54</v>
       </c>
       <c r="E80">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="1">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C81">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D81">
         <v>54</v>
       </c>
       <c r="E81">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="1">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C82">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="D82">
         <v>54</v>
       </c>
       <c r="E82">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="1">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C83">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D83">
         <v>54</v>
       </c>
       <c r="E83">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="1">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B84">
         <v>1</v>
       </c>
       <c r="C84">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="D84">
         <v>54</v>
       </c>
       <c r="E84">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="1">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C85">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D85">
         <v>54</v>
       </c>
       <c r="E85">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="1">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="D86">
         <v>54</v>
       </c>
       <c r="E86">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="1">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C87">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D87">
         <v>54</v>
       </c>
       <c r="E87">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="1">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B88">
         <v>0</v>
       </c>
       <c r="C88">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="D88">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E88">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="1">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D89">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E89">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="1">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B90">
         <v>0</v>
       </c>
       <c r="C90">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D90">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E90">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="1">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B91">
         <v>0</v>
       </c>
       <c r="C91">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="D91">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E91">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="1">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B92">
         <v>0</v>
       </c>
       <c r="C92">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="D92">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E92">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="1">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C93">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="D93">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E93">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="1">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C94">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="D94">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E94">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="1">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C95">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D95">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E95">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="1">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C96">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D96">
         <v>60</v>
       </c>
       <c r="E96">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="1">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C97">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D97">
         <v>60</v>
       </c>
       <c r="E97">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="1">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B98">
         <v>0</v>
       </c>
       <c r="C98">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D98">
         <v>60</v>
       </c>
       <c r="E98">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="1">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C99">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D99">
         <v>60</v>
       </c>
       <c r="E99">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C100">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D100">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E100">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="1">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C101">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D101">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E101">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="1">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C102">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="D102">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E102">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="1">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C103">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D103">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E103">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="1">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C104">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="D104">
         <v>62</v>
       </c>
       <c r="E104">
-        <v>41</v>
+        <v>59</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="1">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C105">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="D105">
         <v>62</v>
       </c>
       <c r="E105">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="1">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B106">
         <v>1</v>
       </c>
       <c r="C106">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D106">
         <v>62</v>
       </c>
       <c r="E106">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="1">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C107">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D107">
         <v>62</v>
       </c>
       <c r="E107">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="1">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C108">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="D108">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E108">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="1">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C109">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="D109">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E109">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="1">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C110">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D110">
         <v>63</v>
       </c>
       <c r="E110">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="1">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B111">
         <v>1</v>
       </c>
       <c r="C111">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="D111">
         <v>63</v>
       </c>
       <c r="E111">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="1">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B112">
         <v>1</v>
       </c>
       <c r="C112">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D112">
         <v>63</v>
       </c>
       <c r="E112">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="1">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C113">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="D113">
         <v>63</v>
       </c>
       <c r="E113">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="1">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C114">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="D114">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E114">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="1">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C115">
         <v>19</v>
       </c>
       <c r="D115">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E115">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="1">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B116">
         <v>0</v>
       </c>
       <c r="C116">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D116">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E116">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="1">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C117">
         <v>19</v>
       </c>
       <c r="D117">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E117">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="1">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B118">
         <v>0</v>
       </c>
       <c r="C118">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D118">
         <v>65</v>
       </c>
       <c r="E118">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="1">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B119">
         <v>0</v>
       </c>
       <c r="C119">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="D119">
         <v>65</v>
       </c>
       <c r="E119">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="1">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B120">
         <v>0</v>
       </c>
       <c r="C120">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="D120">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E120">
         <v>43</v>
@@ -2419,217 +2428,217 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="1">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B121">
         <v>0</v>
       </c>
       <c r="C121">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D121">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E121">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="1">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C122">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="D122">
         <v>67</v>
       </c>
       <c r="E122">
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="1">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B123">
         <v>0</v>
       </c>
       <c r="C123">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D123">
         <v>67</v>
       </c>
       <c r="E123">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="1">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C124">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D124">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E124">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="1">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C125">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D125">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E125">
-        <v>40</v>
+        <v>91</v>
       </c>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="1">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B126">
         <v>0</v>
       </c>
       <c r="C126">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D126">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E126">
-        <v>58</v>
+        <v>29</v>
       </c>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="1">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C127">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D127">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E127">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="1">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B128">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C128">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D128">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E128">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="1">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C129">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D129">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E129">
-        <v>77</v>
+        <v>95</v>
       </c>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="1">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B130">
         <v>1</v>
       </c>
       <c r="C130">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D130">
         <v>71</v>
       </c>
       <c r="E130">
-        <v>35</v>
+        <v>11</v>
       </c>
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="1">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B131">
         <v>1</v>
       </c>
       <c r="C131">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D131">
         <v>71</v>
       </c>
       <c r="E131">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="1">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B132">
         <v>1</v>
       </c>
       <c r="C132">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D132">
         <v>71</v>
       </c>
       <c r="E132">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="1">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B133">
         <v>1</v>
       </c>
       <c r="C133">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D133">
         <v>71</v>
@@ -2640,455 +2649,455 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="1">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C134">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="D134">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E134">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="1">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B135">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C135">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D135">
+        <v>72</v>
+      </c>
+      <c r="E135">
         <v>71</v>
-      </c>
-      <c r="E135">
-        <v>75</v>
       </c>
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="1">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C136">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D136">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E136">
-        <v>34</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="1">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B137">
         <v>0</v>
       </c>
       <c r="C137">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D137">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E137">
-        <v>71</v>
+        <v>88</v>
       </c>
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="1">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B138">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C138">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D138">
         <v>73</v>
       </c>
       <c r="E138">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="1">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C139">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D139">
         <v>73</v>
       </c>
       <c r="E139">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="1">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C140">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="D140">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E140">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="1">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B141">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C141">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D141">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E141">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="1">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B142">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C142">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="D142">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E142">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="1">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B143">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C143">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D143">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E143">
-        <v>72</v>
+        <v>93</v>
       </c>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="1">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B144">
         <v>0</v>
       </c>
       <c r="C144">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="D144">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E144">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="1">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B145">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C145">
         <v>32</v>
       </c>
       <c r="D145">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E145">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="1">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B146">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C146">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D146">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E146">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="1">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C147">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D147">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E147">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="1">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B148">
         <v>1</v>
       </c>
       <c r="C148">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D148">
         <v>77</v>
       </c>
       <c r="E148">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="1">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B149">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C149">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D149">
         <v>77</v>
       </c>
       <c r="E149">
-        <v>97</v>
+        <v>74</v>
       </c>
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="1">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C150">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D150">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E150">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="1">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C151">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D151">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E151">
-        <v>74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="1">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B152">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C152">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D152">
         <v>78</v>
       </c>
       <c r="E152">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="1">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B153">
         <v>1</v>
       </c>
       <c r="C153">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D153">
         <v>78</v>
       </c>
       <c r="E153">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="1">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C154">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D154">
         <v>78</v>
       </c>
       <c r="E154">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="1">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B155">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C155">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D155">
         <v>78</v>
       </c>
       <c r="E155">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="1">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B156">
         <v>0</v>
       </c>
       <c r="C156">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D156">
         <v>78</v>
       </c>
       <c r="E156">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="1">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B157">
         <v>0</v>
       </c>
       <c r="C157">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D157">
         <v>78</v>
       </c>
       <c r="E157">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="1">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C158">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D158">
         <v>78</v>
       </c>
       <c r="E158">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="1">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B159">
         <v>0</v>
       </c>
       <c r="C159">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D159">
         <v>78</v>
       </c>
       <c r="E159">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="1">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B160">
         <v>1</v>
       </c>
       <c r="C160">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D160">
         <v>78</v>
@@ -3099,7 +3108,7 @@
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="1">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -3111,737 +3120,686 @@
         <v>78</v>
       </c>
       <c r="E161">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="1">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B162">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C162">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="D162">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E162">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="1">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B163">
         <v>0</v>
       </c>
       <c r="C163">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D163">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E163">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="1">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B164">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C164">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="D164">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E164">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="1">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B165">
         <v>0</v>
       </c>
       <c r="C165">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D165">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E165">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="1">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B166">
         <v>1</v>
       </c>
       <c r="C166">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="D166">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E166">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="1">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B167">
         <v>0</v>
       </c>
       <c r="C167">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D167">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E167">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="1">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B168">
         <v>1</v>
       </c>
       <c r="C168">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D168">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E168">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="1">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B169">
         <v>0</v>
       </c>
       <c r="C169">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D169">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E169">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="170" spans="1:5">
       <c r="A170" s="1">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B170">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C170">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D170">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E170">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="1">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B171">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C171">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D171">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E171">
-        <v>95</v>
+        <v>63</v>
       </c>
     </row>
     <row r="172" spans="1:5">
       <c r="A172" s="1">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B172">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C172">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D172">
         <v>87</v>
       </c>
       <c r="E172">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="1">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B173">
         <v>1</v>
       </c>
       <c r="C173">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D173">
         <v>87</v>
       </c>
       <c r="E173">
-        <v>63</v>
+        <v>75</v>
       </c>
     </row>
     <row r="174" spans="1:5">
       <c r="A174" s="1">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B174">
         <v>1</v>
       </c>
       <c r="C174">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D174">
         <v>87</v>
       </c>
       <c r="E174">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="1">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B175">
         <v>1</v>
       </c>
       <c r="C175">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D175">
         <v>87</v>
       </c>
       <c r="E175">
-        <v>75</v>
+        <v>92</v>
       </c>
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="1">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B176">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C176">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D176">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E176">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="177" spans="1:5">
       <c r="A177" s="1">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B177">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C177">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D177">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E177">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="178" spans="1:5">
       <c r="A178" s="1">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B178">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C178">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="D178">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E178">
-        <v>44</v>
+        <v>15</v>
       </c>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="1">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B179">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C179">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="D179">
         <v>88</v>
       </c>
       <c r="E179">
-        <v>13</v>
+        <v>69</v>
       </c>
     </row>
     <row r="180" spans="1:5">
       <c r="A180" s="1">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B180">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C180">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D180">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E180">
-        <v>86</v>
+        <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:5">
       <c r="A181" s="1">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B181">
         <v>1</v>
       </c>
       <c r="C181">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D181">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E181">
-        <v>15</v>
+        <v>90</v>
       </c>
     </row>
     <row r="182" spans="1:5">
       <c r="A182" s="1">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B182">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C182">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D182">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E182">
-        <v>69</v>
+        <v>32</v>
       </c>
     </row>
     <row r="183" spans="1:5">
       <c r="A183" s="1">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B183">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C183">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="D183">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E183">
-        <v>14</v>
+        <v>86</v>
       </c>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="1">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B184">
         <v>1</v>
       </c>
       <c r="C184">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D184">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E184">
-        <v>90</v>
+        <v>15</v>
       </c>
     </row>
     <row r="185" spans="1:5">
       <c r="A185" s="1">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B185">
         <v>0</v>
       </c>
       <c r="C185">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D185">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E185">
-        <v>32</v>
+        <v>88</v>
       </c>
     </row>
     <row r="186" spans="1:5">
       <c r="A186" s="1">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B186">
         <v>0</v>
       </c>
       <c r="C186">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D186">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E186">
-        <v>86</v>
+        <v>39</v>
       </c>
     </row>
     <row r="187" spans="1:5">
       <c r="A187" s="1">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B187">
         <v>1</v>
       </c>
       <c r="C187">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D187">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E187">
-        <v>15</v>
+        <v>97</v>
       </c>
     </row>
     <row r="188" spans="1:5">
       <c r="A188" s="1">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B188">
         <v>0</v>
       </c>
       <c r="C188">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D188">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E188">
-        <v>88</v>
+        <v>24</v>
       </c>
     </row>
     <row r="189" spans="1:5">
       <c r="A189" s="1">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B189">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C189">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D189">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E189">
-        <v>39</v>
+        <v>68</v>
       </c>
     </row>
     <row r="190" spans="1:5">
       <c r="A190" s="1">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B190">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C190">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D190">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E190">
-        <v>97</v>
+        <v>17</v>
       </c>
     </row>
     <row r="191" spans="1:5">
       <c r="A191" s="1">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B191">
         <v>0</v>
       </c>
       <c r="C191">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="D191">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E191">
-        <v>24</v>
+        <v>85</v>
       </c>
     </row>
     <row r="192" spans="1:5">
       <c r="A192" s="1">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B192">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C192">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D192">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E192">
-        <v>68</v>
+        <v>23</v>
       </c>
     </row>
     <row r="193" spans="1:5">
       <c r="A193" s="1">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B193">
         <v>0</v>
       </c>
       <c r="C193">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D193">
         <v>103</v>
       </c>
       <c r="E193">
-        <v>17</v>
+        <v>69</v>
       </c>
     </row>
     <row r="194" spans="1:5">
       <c r="A194" s="1">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B194">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C194">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D194">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E194">
-        <v>85</v>
+        <v>8</v>
       </c>
     </row>
     <row r="195" spans="1:5">
       <c r="A195" s="1">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B195">
         <v>0</v>
       </c>
       <c r="C195">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D195">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E195">
-        <v>23</v>
+        <v>91</v>
       </c>
     </row>
     <row r="196" spans="1:5">
       <c r="A196" s="1">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B196">
         <v>0</v>
       </c>
       <c r="C196">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D196">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="E196">
-        <v>69</v>
+        <v>16</v>
       </c>
     </row>
     <row r="197" spans="1:5">
       <c r="A197" s="1">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B197">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C197">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D197">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="E197">
-        <v>8</v>
+        <v>79</v>
       </c>
     </row>
     <row r="198" spans="1:5">
       <c r="A198" s="1">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B198">
         <v>0</v>
       </c>
       <c r="C198">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D198">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="E198">
-        <v>91</v>
+        <v>28</v>
       </c>
     </row>
     <row r="199" spans="1:5">
       <c r="A199" s="1">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B199">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C199">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D199">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E199">
-        <v>16</v>
+        <v>74</v>
       </c>
     </row>
     <row r="200" spans="1:5">
       <c r="A200" s="1">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B200">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C200">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D200">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="E200">
-        <v>79</v>
+        <v>18</v>
       </c>
     </row>
     <row r="201" spans="1:5">
       <c r="A201" s="1">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B201">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C201">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D201">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="E201">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5">
-      <c r="A202" s="1">
-        <v>200</v>
-      </c>
-      <c r="B202">
-        <v>1</v>
-      </c>
-      <c r="C202">
-        <v>32</v>
-      </c>
-      <c r="D202">
-        <v>126</v>
-      </c>
-      <c r="E202">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5">
-      <c r="A203" s="1">
-        <v>201</v>
-      </c>
-      <c r="B203">
-        <v>1</v>
-      </c>
-      <c r="C203">
-        <v>32</v>
-      </c>
-      <c r="D203">
-        <v>137</v>
-      </c>
-      <c r="E203">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5">
-      <c r="A204" s="1">
-        <v>202</v>
-      </c>
-      <c r="B204">
-        <v>1</v>
-      </c>
-      <c r="C204">
-        <v>30</v>
-      </c>
-      <c r="D204">
-        <v>137</v>
-      </c>
-      <c r="E204">
         <v>83</v>
       </c>
     </row>

</xml_diff>